<commit_message>
Fix bug with BusinessEntity_ID format and update README
</commit_message>
<xml_diff>
--- a/data/Colorado-Breweries.xlsx
+++ b/data/Colorado-Breweries.xlsx
@@ -24,6 +24,7 @@
   </externalReferences>
   <definedNames>
     <definedName name="BasinChoices">[1]IBCC_Basin!$A$5:$A$13</definedName>
+    <definedName name="Book3" localSheetId="1">Brewery!#REF!</definedName>
     <definedName name="CountyChoices" localSheetId="3">[2]County!$A$5:$A$69</definedName>
     <definedName name="CountyChoices">[1]County!$A$5:$A$68</definedName>
     <definedName name="GeocodeAddressColumn_BeerBeerBeer">#REF!</definedName>
@@ -393,7 +394,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="623" uniqueCount="206">
   <si>
     <t>When</t>
   </si>
@@ -1206,6 +1207,54 @@
   <si>
     <t>This dataset began as a list of breweries operating in or near Fort Collins, provided by an article (https://www.coloradoan.com/story/life/food/beer/2017/12/30/fort-collins-brewery-scene-still-growing-2018/966966001/) from the Fort Collins Coloradoan newspaper.  The article also listed the year in which the brewery opened, which was used for breweries without a BusinessEntity_ID and the Anheuser-Busch and C.B. and Potts breweries, since this information was not clear from the other sources described below.</t>
   </si>
+  <si>
+    <t>19871090304</t>
+  </si>
+  <si>
+    <t>20101029498</t>
+  </si>
+  <si>
+    <t>19891008581</t>
+  </si>
+  <si>
+    <t>19891038227</t>
+  </si>
+  <si>
+    <t>19931026399</t>
+  </si>
+  <si>
+    <t>20091520154</t>
+  </si>
+  <si>
+    <t>20091511612</t>
+  </si>
+  <si>
+    <t>20101237661</t>
+  </si>
+  <si>
+    <t>20131106452</t>
+  </si>
+  <si>
+    <t>20111663628</t>
+  </si>
+  <si>
+    <t>20131455057</t>
+  </si>
+  <si>
+    <t>20131223376</t>
+  </si>
+  <si>
+    <t>20141532224</t>
+  </si>
+  <si>
+    <t>20141790998</t>
+  </si>
+  <si>
+    <t>20161542027</t>
+  </si>
+  <si>
+    <t>20131179458</t>
+  </si>
 </sst>
 </file>
 
@@ -1213,9 +1262,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
-    <numFmt numFmtId="169" formatCode="0.000000"/>
+    <numFmt numFmtId="165" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1257,11 +1306,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Raleway"/>
     </font>
     <font>
       <u/>
@@ -1337,9 +1381,9 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1357,9 +1401,8 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1377,19 +1420,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="169" fontId="8" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -1398,6 +1435,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -1405,6 +1445,22 @@
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
   <dxfs count="18">
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1417,18 +1473,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -1450,7 +1494,7 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="169" formatCode="0.000000"/>
+      <numFmt numFmtId="165" formatCode="0.000000"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -1475,7 +1519,7 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="169" formatCode="0.000000"/>
+      <numFmt numFmtId="165" formatCode="0.000000"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1500,7 +1544,7 @@
         <name val="Calibri"/>
         <scheme val="none"/>
       </font>
-      <numFmt numFmtId="169" formatCode="0.000000"/>
+      <numFmt numFmtId="165" formatCode="0.000000"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1543,13 +1587,9 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2377,33 +2417,33 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:X23" totalsRowShown="0" headerRowDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:X23" totalsRowShown="0" headerRowDxfId="17">
   <autoFilter ref="A1:X23"/>
   <tableColumns count="24">
     <tableColumn id="1" name="BreweryName"/>
     <tableColumn id="2" name="OWF_ID"/>
-    <tableColumn id="3" name="OWF_ID_Flag" dataDxfId="17"/>
-    <tableColumn id="4" name="BusinessEntity_ID" dataDxfId="16"/>
-    <tableColumn id="5" name="BusinessEntity_ID_Flag" dataDxfId="15"/>
+    <tableColumn id="3" name="OWF_ID_Flag" dataDxfId="16"/>
+    <tableColumn id="25" name="BusinessEntity_ID" dataDxfId="0"/>
+    <tableColumn id="5" name="BusinessEntity_ID_Flag" dataDxfId="1"/>
     <tableColumn id="6" name="Physical_ Address"/>
     <tableColumn id="7" name="Municipality"/>
     <tableColumn id="8" name="State"/>
-    <tableColumn id="9" name="ZipCode" dataDxfId="0"/>
-    <tableColumn id="10" name="Municipality_DOLA_LG_ID" dataDxfId="1"/>
-    <tableColumn id="11" name="Municipality_DOLA_LG_ID_Flag" dataDxfId="14"/>
-    <tableColumn id="12" name="Municipal_WaterProvider_OWF_ID" dataDxfId="13" dataCellStyle="Normal 2"/>
-    <tableColumn id="13" name="Municipal_WaterProvider_OWF_ID_Flag" dataDxfId="12"/>
-    <tableColumn id="14" name="Latitude" dataDxfId="11"/>
-    <tableColumn id="15" name="Longitude" dataDxfId="10"/>
-    <tableColumn id="16" name="Lat_Long_Flag" dataDxfId="9"/>
+    <tableColumn id="9" name="ZipCode" dataDxfId="15"/>
+    <tableColumn id="10" name="Municipality_DOLA_LG_ID" dataDxfId="14"/>
+    <tableColumn id="11" name="Municipality_DOLA_LG_ID_Flag" dataDxfId="13"/>
+    <tableColumn id="12" name="Municipal_WaterProvider_OWF_ID" dataDxfId="12" dataCellStyle="Normal 2"/>
+    <tableColumn id="13" name="Municipal_WaterProvider_OWF_ID_Flag" dataDxfId="11"/>
+    <tableColumn id="14" name="Latitude" dataDxfId="10"/>
+    <tableColumn id="15" name="Longitude" dataDxfId="9"/>
+    <tableColumn id="16" name="Lat_Long_Flag" dataDxfId="8"/>
     <tableColumn id="17" name="WaterSource_GNIS_Name"/>
-    <tableColumn id="18" name="WaterSource_GNIS_Name_Flag" dataDxfId="4"/>
-    <tableColumn id="19" name="WaterSource_GNIS_ID" dataDxfId="2"/>
-    <tableColumn id="20" name="WaterSource_GNIS_ID_Flag" dataDxfId="3"/>
+    <tableColumn id="18" name="WaterSource_GNIS_Name_Flag" dataDxfId="7"/>
+    <tableColumn id="19" name="WaterSource_GNIS_ID" dataDxfId="6"/>
+    <tableColumn id="20" name="WaterSource_GNIS_ID_Flag" dataDxfId="5"/>
     <tableColumn id="21" name="Website" dataCellStyle="Hyperlink"/>
-    <tableColumn id="22" name="Website_Flag" dataDxfId="7"/>
-    <tableColumn id="23" name="Formation_Year" dataDxfId="5"/>
-    <tableColumn id="24" name="Formation_Year_Flag" dataDxfId="6"/>
+    <tableColumn id="22" name="Website_Flag" dataDxfId="4"/>
+    <tableColumn id="23" name="Formation_Year" dataDxfId="3"/>
+    <tableColumn id="24" name="Formation_Year_Flag" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2678,144 +2718,144 @@
       <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="173.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="22" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="45">
-      <c r="A2" s="17" t="s">
+    <row r="2" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
-      <c r="A3" s="17"/>
-    </row>
-    <row r="4" spans="1:1" ht="45">
-      <c r="A4" s="17" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="16"/>
+    </row>
+    <row r="4" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
-      <c r="A5" s="17"/>
-    </row>
-    <row r="6" spans="1:1" ht="45">
-      <c r="A6" s="17" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="16"/>
+    </row>
+    <row r="6" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="17"/>
-    </row>
-    <row r="8" spans="1:1" ht="30">
-      <c r="A8" s="17" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="16"/>
+    </row>
+    <row r="8" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
-      <c r="A9" s="17"/>
-    </row>
-    <row r="10" spans="1:1" ht="45">
-      <c r="A10" s="16" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="16"/>
+    </row>
+    <row r="10" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
-      <c r="A11" s="16"/>
-    </row>
-    <row r="12" spans="1:1" ht="45">
-      <c r="A12" s="16" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="15"/>
+    </row>
+    <row r="12" spans="1:1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
-      <c r="A13" s="16"/>
-    </row>
-    <row r="14" spans="1:1" ht="30">
-      <c r="A14" s="16" t="s">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="15"/>
+    </row>
+    <row r="14" spans="1:1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="15" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
-      <c r="A15" s="16"/>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16" s="25" t="s">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="15"/>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="22" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="24" t="s">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="21" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
-      <c r="A18" s="24" t="s">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="21" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
-      <c r="A19" s="24" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="21" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
-      <c r="A20" s="24" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="21" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
-      <c r="A21" s="24" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="21" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
-      <c r="A22" s="24" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="21" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
-      <c r="A23" s="16" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="15" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
-      <c r="A24" s="16" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="15" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="5"/>
     </row>
-    <row r="26" spans="1:1">
-      <c r="A26" s="25" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="22" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
     </row>
-    <row r="29" spans="1:1">
-      <c r="A29" s="25" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="22" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="5"/>
     </row>
   </sheetData>
@@ -2825,21 +2865,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X30"/>
+  <dimension ref="A1:X24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B25" sqref="B25"/>
+      <selection pane="bottomRight" activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.42578125" customWidth="1"/>
     <col min="5" max="5" width="26.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.140625" customWidth="1"/>
     <col min="7" max="7" width="16.7109375" bestFit="1" customWidth="1"/>
@@ -2862,7 +2902,7 @@
     <col min="24" max="24" width="24.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -2936,7 +2976,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -2946,10 +2986,10 @@
       <c r="C2" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="19">
-        <v>19871090304</v>
-      </c>
-      <c r="E2" s="18" t="s">
+      <c r="D2" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="E2" s="17" t="s">
         <v>45</v>
       </c>
       <c r="F2" s="7" t="s">
@@ -2961,7 +3001,7 @@
       <c r="H2" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="I2" s="15">
+      <c r="I2" s="14">
         <v>80524</v>
       </c>
       <c r="J2" s="6" t="s">
@@ -2970,19 +3010,19 @@
       <c r="K2" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="L2" s="15" t="s">
+      <c r="L2" s="14" t="s">
         <v>130</v>
       </c>
       <c r="M2" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="N2" s="23">
+      <c r="N2" s="20">
         <v>40.617477000000001</v>
       </c>
-      <c r="O2" s="23">
+      <c r="O2" s="20">
         <v>-105.0051165</v>
       </c>
-      <c r="P2" s="22" t="s">
+      <c r="P2" s="19" t="s">
         <v>173</v>
       </c>
       <c r="Q2" t="s">
@@ -2991,10 +3031,10 @@
       <c r="R2" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="S2" s="20" t="s">
+      <c r="S2" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="T2" s="20" t="s">
+      <c r="T2" s="18" t="s">
         <v>45</v>
       </c>
       <c r="U2" s="8" t="s">
@@ -3010,7 +3050,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -3020,10 +3060,10 @@
       <c r="C3" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="19">
-        <v>20101029498</v>
-      </c>
-      <c r="E3" s="18" t="s">
+      <c r="D3" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="E3" s="17" t="s">
         <v>45</v>
       </c>
       <c r="F3" s="7" t="s">
@@ -3035,7 +3075,7 @@
       <c r="H3" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="I3" s="15">
+      <c r="I3" s="14">
         <v>80525</v>
       </c>
       <c r="J3" s="6" t="s">
@@ -3044,19 +3084,19 @@
       <c r="K3" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="L3" s="15" t="s">
+      <c r="L3" s="14" t="s">
         <v>130</v>
       </c>
       <c r="M3" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="N3" s="23">
+      <c r="N3" s="20">
         <v>40.537612600000003</v>
       </c>
-      <c r="O3" s="23">
+      <c r="O3" s="20">
         <v>-105.0509615</v>
       </c>
-      <c r="P3" s="22" t="s">
+      <c r="P3" s="19" t="s">
         <v>173</v>
       </c>
       <c r="Q3" t="s">
@@ -3065,10 +3105,10 @@
       <c r="R3" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="S3" s="20" t="s">
+      <c r="S3" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="T3" s="20" t="s">
+      <c r="T3" s="18" t="s">
         <v>45</v>
       </c>
       <c r="U3" s="8" t="s">
@@ -3084,7 +3124,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>122</v>
       </c>
@@ -3094,10 +3134,10 @@
       <c r="C4" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="20">
-        <v>19891008581</v>
-      </c>
-      <c r="E4" s="18" t="s">
+      <c r="D4" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="E4" s="17" t="s">
         <v>45</v>
       </c>
       <c r="F4" t="s">
@@ -3118,19 +3158,19 @@
       <c r="K4" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="L4" s="15" t="s">
+      <c r="L4" s="14" t="s">
         <v>130</v>
       </c>
       <c r="M4" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="N4" s="23">
+      <c r="N4" s="20">
         <v>40.587408799999999</v>
       </c>
-      <c r="O4" s="23">
+      <c r="O4" s="20">
         <v>-105.07565459999999</v>
       </c>
-      <c r="P4" s="22" t="s">
+      <c r="P4" s="19" t="s">
         <v>173</v>
       </c>
       <c r="Q4" t="s">
@@ -3139,10 +3179,10 @@
       <c r="R4" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="S4" s="20" t="s">
+      <c r="S4" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="T4" s="20" t="s">
+      <c r="T4" s="18" t="s">
         <v>45</v>
       </c>
       <c r="U4" s="8" t="s">
@@ -3158,7 +3198,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>65</v>
       </c>
@@ -3168,10 +3208,10 @@
       <c r="C5" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D5" s="20">
-        <v>19891038227</v>
-      </c>
-      <c r="E5" s="18" t="s">
+      <c r="D5" s="18" t="s">
+        <v>193</v>
+      </c>
+      <c r="E5" s="17" t="s">
         <v>45</v>
       </c>
       <c r="F5" t="s">
@@ -3192,19 +3232,19 @@
       <c r="K5" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="L5" s="15" t="s">
+      <c r="L5" s="14" t="s">
         <v>130</v>
       </c>
       <c r="M5" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="N5" s="23">
+      <c r="N5" s="20">
         <v>40.589467399999997</v>
       </c>
-      <c r="O5" s="23">
+      <c r="O5" s="20">
         <v>-105.0631819</v>
       </c>
-      <c r="P5" s="22" t="s">
+      <c r="P5" s="19" t="s">
         <v>173</v>
       </c>
       <c r="Q5" t="s">
@@ -3213,10 +3253,10 @@
       <c r="R5" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="S5" s="20" t="s">
+      <c r="S5" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="T5" s="20" t="s">
+      <c r="T5" s="18" t="s">
         <v>45</v>
       </c>
       <c r="U5" s="8" t="s">
@@ -3232,7 +3272,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>92</v>
       </c>
@@ -3242,10 +3282,10 @@
       <c r="C6" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D6" s="20">
-        <v>19931026399</v>
-      </c>
-      <c r="E6" s="18" t="s">
+      <c r="D6" s="18" t="s">
+        <v>194</v>
+      </c>
+      <c r="E6" s="17" t="s">
         <v>45</v>
       </c>
       <c r="F6" t="s">
@@ -3266,19 +3306,19 @@
       <c r="K6" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="L6" s="15" t="s">
+      <c r="L6" s="14" t="s">
         <v>130</v>
       </c>
       <c r="M6" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="N6" s="23">
+      <c r="N6" s="20">
         <v>40.593493799999997</v>
       </c>
-      <c r="O6" s="23">
+      <c r="O6" s="20">
         <v>-104.9676006</v>
       </c>
-      <c r="P6" s="22" t="s">
+      <c r="P6" s="19" t="s">
         <v>173</v>
       </c>
       <c r="Q6" t="s">
@@ -3287,10 +3327,10 @@
       <c r="R6" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="S6" s="20" t="s">
+      <c r="S6" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="T6" s="20" t="s">
+      <c r="T6" s="18" t="s">
         <v>45</v>
       </c>
       <c r="U6" s="8" t="s">
@@ -3306,7 +3346,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="7" spans="1:24">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>93</v>
       </c>
@@ -3316,10 +3356,10 @@
       <c r="C7" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D7" s="20">
-        <v>20091520154</v>
-      </c>
-      <c r="E7" s="18" t="s">
+      <c r="D7" s="18" t="s">
+        <v>195</v>
+      </c>
+      <c r="E7" s="17" t="s">
         <v>45</v>
       </c>
       <c r="F7" t="s">
@@ -3340,19 +3380,19 @@
       <c r="K7" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="L7" s="15" t="s">
+      <c r="L7" s="14" t="s">
         <v>130</v>
       </c>
       <c r="M7" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="N7" s="23">
+      <c r="N7" s="20">
         <v>40.586344199999999</v>
       </c>
-      <c r="O7" s="23">
+      <c r="O7" s="20">
         <v>-105.07582960000001</v>
       </c>
-      <c r="P7" s="22" t="s">
+      <c r="P7" s="19" t="s">
         <v>173</v>
       </c>
       <c r="Q7" t="s">
@@ -3361,10 +3401,10 @@
       <c r="R7" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="S7" s="20" t="s">
+      <c r="S7" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="T7" s="20" t="s">
+      <c r="T7" s="18" t="s">
         <v>45</v>
       </c>
       <c r="U7" s="8" t="s">
@@ -3380,7 +3420,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="8" spans="1:24">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>32</v>
       </c>
@@ -3390,10 +3430,10 @@
       <c r="C8" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D8" s="19">
-        <v>20091511612</v>
-      </c>
-      <c r="E8" s="18" t="s">
+      <c r="D8" s="18" t="s">
+        <v>196</v>
+      </c>
+      <c r="E8" s="17" t="s">
         <v>45</v>
       </c>
       <c r="F8" s="7" t="s">
@@ -3405,7 +3445,7 @@
       <c r="H8" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="I8" s="15">
+      <c r="I8" s="14">
         <v>80524</v>
       </c>
       <c r="J8" s="6" t="s">
@@ -3414,19 +3454,19 @@
       <c r="K8" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="L8" s="15" t="s">
+      <c r="L8" s="14" t="s">
         <v>130</v>
       </c>
       <c r="M8" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="N8" s="23">
+      <c r="N8" s="20">
         <v>40.583198600000003</v>
       </c>
-      <c r="O8" s="23">
+      <c r="O8" s="20">
         <v>-105.0421247</v>
       </c>
-      <c r="P8" s="22" t="s">
+      <c r="P8" s="19" t="s">
         <v>173</v>
       </c>
       <c r="Q8" t="s">
@@ -3435,10 +3475,10 @@
       <c r="R8" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="S8" s="20" t="s">
+      <c r="S8" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="T8" s="20" t="s">
+      <c r="T8" s="18" t="s">
         <v>45</v>
       </c>
       <c r="U8" s="8" t="s">
@@ -3454,7 +3494,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="9" spans="1:24">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>33</v>
       </c>
@@ -3464,10 +3504,10 @@
       <c r="C9" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D9" s="20">
-        <v>20101237661</v>
-      </c>
-      <c r="E9" s="18" t="s">
+      <c r="D9" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="E9" s="17" t="s">
         <v>45</v>
       </c>
       <c r="F9" t="s">
@@ -3488,19 +3528,19 @@
       <c r="K9" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="L9" s="15" t="s">
+      <c r="L9" s="14" t="s">
         <v>130</v>
       </c>
       <c r="M9" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="N9" s="23">
+      <c r="N9" s="20">
         <v>40.566196499999997</v>
       </c>
-      <c r="O9" s="23">
+      <c r="O9" s="20">
         <v>-105.0786153</v>
       </c>
-      <c r="P9" s="22" t="s">
+      <c r="P9" s="19" t="s">
         <v>173</v>
       </c>
       <c r="Q9" t="s">
@@ -3509,13 +3549,13 @@
       <c r="R9" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="S9" s="20" t="s">
+      <c r="S9" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="T9" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="U9" s="10" t="s">
+      <c r="T9" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="U9" s="9" t="s">
         <v>55</v>
       </c>
       <c r="V9" s="6" t="s">
@@ -3528,7 +3568,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="10" spans="1:24">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>72</v>
       </c>
@@ -3538,7 +3578,7 @@
       <c r="C10" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D10" s="21"/>
+      <c r="D10" s="23"/>
       <c r="E10" s="6" t="s">
         <v>140</v>
       </c>
@@ -3560,19 +3600,19 @@
       <c r="K10" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="L10" s="15" t="s">
+      <c r="L10" s="14" t="s">
         <v>130</v>
       </c>
       <c r="M10" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="N10" s="23">
+      <c r="N10" s="20">
         <v>40.553051699999997</v>
       </c>
-      <c r="O10" s="23">
+      <c r="O10" s="20">
         <v>-105.0973809</v>
       </c>
-      <c r="P10" s="22" t="s">
+      <c r="P10" s="19" t="s">
         <v>173</v>
       </c>
       <c r="Q10" t="s">
@@ -3581,10 +3621,10 @@
       <c r="R10" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="S10" s="20" t="s">
+      <c r="S10" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="T10" s="20" t="s">
+      <c r="T10" s="18" t="s">
         <v>45</v>
       </c>
       <c r="U10" t="s">
@@ -3600,7 +3640,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="11" spans="1:24">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>94</v>
       </c>
@@ -3610,10 +3650,10 @@
       <c r="C11" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D11" s="20">
-        <v>20131106452</v>
-      </c>
-      <c r="E11" s="18" t="s">
+      <c r="D11" s="18" t="s">
+        <v>198</v>
+      </c>
+      <c r="E11" s="17" t="s">
         <v>45</v>
       </c>
       <c r="F11" t="s">
@@ -3634,19 +3674,19 @@
       <c r="K11" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="L11" s="15" t="s">
+      <c r="L11" s="14" t="s">
         <v>130</v>
       </c>
       <c r="M11" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="N11" s="23">
+      <c r="N11" s="20">
         <v>40.589680399999999</v>
       </c>
-      <c r="O11" s="23">
+      <c r="O11" s="20">
         <v>-105.045597</v>
       </c>
-      <c r="P11" s="22" t="s">
+      <c r="P11" s="19" t="s">
         <v>173</v>
       </c>
       <c r="Q11" t="s">
@@ -3655,10 +3695,10 @@
       <c r="R11" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="S11" s="20" t="s">
+      <c r="S11" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="T11" s="20" t="s">
+      <c r="T11" s="18" t="s">
         <v>45</v>
       </c>
       <c r="U11" s="8" t="s">
@@ -3674,7 +3714,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="12" spans="1:24">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>41</v>
       </c>
@@ -3684,10 +3724,10 @@
       <c r="C12" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D12" s="20">
-        <v>20111663628</v>
-      </c>
-      <c r="E12" s="18" t="s">
+      <c r="D12" s="18" t="s">
+        <v>199</v>
+      </c>
+      <c r="E12" s="17" t="s">
         <v>45</v>
       </c>
       <c r="F12" t="s">
@@ -3708,19 +3748,19 @@
       <c r="K12" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="L12" s="15" t="s">
+      <c r="L12" s="14" t="s">
         <v>130</v>
       </c>
       <c r="M12" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="N12" s="23">
+      <c r="N12" s="20">
         <v>40.589933600000002</v>
       </c>
-      <c r="O12" s="23">
+      <c r="O12" s="20">
         <v>-105.0584095</v>
       </c>
-      <c r="P12" s="22" t="s">
+      <c r="P12" s="19" t="s">
         <v>173</v>
       </c>
       <c r="Q12" t="s">
@@ -3729,10 +3769,10 @@
       <c r="R12" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="S12" s="20" t="s">
+      <c r="S12" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="T12" s="20" t="s">
+      <c r="T12" s="18" t="s">
         <v>45</v>
       </c>
       <c r="U12" s="8" t="s">
@@ -3748,7 +3788,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="13" spans="1:24">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>34</v>
       </c>
@@ -3758,7 +3798,7 @@
       <c r="C13" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D13" s="21"/>
+      <c r="D13" s="23"/>
       <c r="E13" s="6" t="s">
         <v>140</v>
       </c>
@@ -3780,19 +3820,19 @@
       <c r="K13" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="L13" s="15" t="s">
+      <c r="L13" s="14" t="s">
         <v>130</v>
       </c>
       <c r="M13" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="N13" s="23">
+      <c r="N13" s="20">
         <v>40.522753100000003</v>
       </c>
-      <c r="O13" s="23">
+      <c r="O13" s="20">
         <v>-105.07836</v>
       </c>
-      <c r="P13" s="22" t="s">
+      <c r="P13" s="19" t="s">
         <v>173</v>
       </c>
       <c r="Q13" t="s">
@@ -3801,10 +3841,10 @@
       <c r="R13" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="S13" s="20" t="s">
+      <c r="S13" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="T13" s="20" t="s">
+      <c r="T13" s="18" t="s">
         <v>45</v>
       </c>
       <c r="U13" s="8" t="s">
@@ -3820,7 +3860,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="14" spans="1:24">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>35</v>
       </c>
@@ -3830,10 +3870,10 @@
       <c r="C14" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D14" s="20">
-        <v>20131455057</v>
-      </c>
-      <c r="E14" s="18" t="s">
+      <c r="D14" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="E14" s="17" t="s">
         <v>45</v>
       </c>
       <c r="F14" t="s">
@@ -3854,19 +3894,19 @@
       <c r="K14" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="L14" s="15" t="s">
+      <c r="L14" s="14" t="s">
         <v>130</v>
       </c>
       <c r="M14" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="N14" s="23">
+      <c r="N14" s="20">
         <v>40.566066599999999</v>
       </c>
-      <c r="O14" s="23">
+      <c r="O14" s="20">
         <v>-105.0567044</v>
       </c>
-      <c r="P14" s="22" t="s">
+      <c r="P14" s="19" t="s">
         <v>173</v>
       </c>
       <c r="Q14" t="s">
@@ -3875,13 +3915,13 @@
       <c r="R14" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="S14" s="20" t="s">
+      <c r="S14" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="T14" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="U14" s="11" t="s">
+      <c r="T14" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="U14" s="10" t="s">
         <v>81</v>
       </c>
       <c r="V14" s="6" t="s">
@@ -3894,7 +3934,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="15" spans="1:24">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>46</v>
       </c>
@@ -3904,10 +3944,10 @@
       <c r="C15" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D15" s="20">
-        <v>20131223376</v>
-      </c>
-      <c r="E15" s="18" t="s">
+      <c r="D15" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="E15" s="17" t="s">
         <v>45</v>
       </c>
       <c r="F15" t="s">
@@ -3928,19 +3968,19 @@
       <c r="K15" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="L15" s="15" t="s">
+      <c r="L15" s="14" t="s">
         <v>130</v>
       </c>
       <c r="M15" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="N15" s="23">
+      <c r="N15" s="20">
         <v>40.583178400000001</v>
       </c>
-      <c r="O15" s="23">
+      <c r="O15" s="20">
         <v>-105.0680043</v>
       </c>
-      <c r="P15" s="22" t="s">
+      <c r="P15" s="19" t="s">
         <v>173</v>
       </c>
       <c r="Q15" t="s">
@@ -3949,13 +3989,13 @@
       <c r="R15" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="S15" s="20" t="s">
+      <c r="S15" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="T15" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="U15" s="11" t="s">
+      <c r="T15" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="U15" s="10" t="s">
         <v>82</v>
       </c>
       <c r="V15" s="6" t="s">
@@ -3968,7 +4008,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="16" spans="1:24">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>95</v>
       </c>
@@ -3978,10 +4018,10 @@
       <c r="C16" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D16" s="19">
-        <v>20141532224</v>
-      </c>
-      <c r="E16" s="18" t="s">
+      <c r="D16" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="E16" s="17" t="s">
         <v>45</v>
       </c>
       <c r="F16" t="s">
@@ -4002,19 +4042,19 @@
       <c r="K16" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="L16" s="15" t="s">
+      <c r="L16" s="14" t="s">
         <v>130</v>
       </c>
       <c r="M16" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="N16" s="23">
+      <c r="N16" s="20">
         <v>40.572846200000001</v>
       </c>
-      <c r="O16" s="23">
+      <c r="O16" s="20">
         <v>-105.11539759999999</v>
       </c>
-      <c r="P16" s="22" t="s">
+      <c r="P16" s="19" t="s">
         <v>173</v>
       </c>
       <c r="Q16" t="s">
@@ -4023,13 +4063,13 @@
       <c r="R16" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="S16" s="20" t="s">
+      <c r="S16" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="T16" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="U16" s="11" t="s">
+      <c r="T16" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="U16" s="10" t="s">
         <v>77</v>
       </c>
       <c r="V16" s="6" t="s">
@@ -4042,7 +4082,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="17" spans="1:24">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>96</v>
       </c>
@@ -4052,10 +4092,10 @@
       <c r="C17" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D17" s="19">
-        <v>20141790998</v>
-      </c>
-      <c r="E17" s="18" t="s">
+      <c r="D17" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="E17" s="17" t="s">
         <v>45</v>
       </c>
       <c r="F17" t="s">
@@ -4076,19 +4116,19 @@
       <c r="K17" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="L17" s="15" t="s">
+      <c r="L17" s="14" t="s">
         <v>130</v>
       </c>
       <c r="M17" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="N17" s="23">
+      <c r="N17" s="20">
         <v>40.575092400000003</v>
       </c>
-      <c r="O17" s="23">
+      <c r="O17" s="20">
         <v>-105.0966413</v>
       </c>
-      <c r="P17" s="22" t="s">
+      <c r="P17" s="19" t="s">
         <v>173</v>
       </c>
       <c r="Q17" t="s">
@@ -4097,13 +4137,13 @@
       <c r="R17" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="S17" s="20" t="s">
+      <c r="S17" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="T17" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="U17" s="11" t="s">
+      <c r="T17" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="U17" s="10" t="s">
         <v>76</v>
       </c>
       <c r="V17" s="6" t="s">
@@ -4116,7 +4156,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="18" spans="1:24">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -4126,7 +4166,7 @@
       <c r="C18" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D18" s="21"/>
+      <c r="D18" s="23"/>
       <c r="E18" s="6" t="s">
         <v>140</v>
       </c>
@@ -4148,19 +4188,19 @@
       <c r="K18" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="L18" s="15" t="s">
+      <c r="L18" s="14" t="s">
         <v>130</v>
       </c>
       <c r="M18" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="N18" s="23">
+      <c r="N18" s="20">
         <v>40.562033200000002</v>
       </c>
-      <c r="O18" s="23">
+      <c r="O18" s="20">
         <v>-105.0380159</v>
       </c>
-      <c r="P18" s="22" t="s">
+      <c r="P18" s="19" t="s">
         <v>173</v>
       </c>
       <c r="Q18" t="s">
@@ -4169,10 +4209,10 @@
       <c r="R18" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="S18" s="20" t="s">
+      <c r="S18" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="T18" s="20" t="s">
+      <c r="T18" s="18" t="s">
         <v>45</v>
       </c>
       <c r="U18" t="s">
@@ -4188,7 +4228,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="19" spans="1:24">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>37</v>
       </c>
@@ -4198,7 +4238,7 @@
       <c r="C19" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D19" s="21"/>
+      <c r="D19" s="23"/>
       <c r="E19" s="6" t="s">
         <v>140</v>
       </c>
@@ -4220,19 +4260,19 @@
       <c r="K19" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="L19" s="15" t="s">
+      <c r="L19" s="14" t="s">
         <v>130</v>
       </c>
       <c r="M19" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="N19" s="23">
+      <c r="N19" s="20">
         <v>40.550711200000002</v>
       </c>
-      <c r="O19" s="23">
+      <c r="O19" s="20">
         <v>-105.0798466</v>
       </c>
-      <c r="P19" s="22" t="s">
+      <c r="P19" s="19" t="s">
         <v>173</v>
       </c>
       <c r="Q19" t="s">
@@ -4241,13 +4281,13 @@
       <c r="R19" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="S19" s="20" t="s">
+      <c r="S19" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="T19" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="U19" s="11" t="s">
+      <c r="T19" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="U19" s="10" t="s">
         <v>83</v>
       </c>
       <c r="V19" s="6" t="s">
@@ -4260,7 +4300,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="20" spans="1:24">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -4270,7 +4310,7 @@
       <c r="C20" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D20" s="21"/>
+      <c r="D20" s="23"/>
       <c r="E20" s="6" t="s">
         <v>140</v>
       </c>
@@ -4292,19 +4332,19 @@
       <c r="K20" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="L20" s="15" t="s">
+      <c r="L20" s="14" t="s">
         <v>130</v>
       </c>
       <c r="M20" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="N20" s="23">
+      <c r="N20" s="20">
         <v>40.5545197</v>
       </c>
-      <c r="O20" s="23">
+      <c r="O20" s="20">
         <v>-105.1166484</v>
       </c>
-      <c r="P20" s="22" t="s">
+      <c r="P20" s="19" t="s">
         <v>173</v>
       </c>
       <c r="Q20" t="s">
@@ -4313,13 +4353,13 @@
       <c r="R20" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="S20" s="20" t="s">
+      <c r="S20" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="T20" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="U20" s="11" t="s">
+      <c r="T20" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="U20" s="10" t="s">
         <v>85</v>
       </c>
       <c r="V20" s="6" t="s">
@@ -4332,7 +4372,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="21" spans="1:24">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>97</v>
       </c>
@@ -4342,7 +4382,7 @@
       <c r="C21" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="21"/>
+      <c r="D21" s="23"/>
       <c r="E21" s="6" t="s">
         <v>140</v>
       </c>
@@ -4364,19 +4404,19 @@
       <c r="K21" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="L21" s="15" t="s">
+      <c r="L21" s="14" t="s">
         <v>130</v>
       </c>
       <c r="M21" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="N21" s="23">
+      <c r="N21" s="20">
         <v>40.539290299999998</v>
       </c>
-      <c r="O21" s="23">
+      <c r="O21" s="20">
         <v>-105.0752914</v>
       </c>
-      <c r="P21" s="22" t="s">
+      <c r="P21" s="19" t="s">
         <v>173</v>
       </c>
       <c r="Q21" t="s">
@@ -4385,13 +4425,13 @@
       <c r="R21" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="S21" s="20" t="s">
+      <c r="S21" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="T21" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="U21" s="11" t="s">
+      <c r="T21" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="U21" s="10" t="s">
         <v>87</v>
       </c>
       <c r="V21" s="6" t="s">
@@ -4404,7 +4444,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="22" spans="1:24">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>39</v>
       </c>
@@ -4414,10 +4454,10 @@
       <c r="C22" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D22" s="19">
-        <v>20161542027</v>
-      </c>
-      <c r="E22" s="18" t="s">
+      <c r="D22" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="E22" s="17" t="s">
         <v>45</v>
       </c>
       <c r="F22" t="s">
@@ -4438,19 +4478,19 @@
       <c r="K22" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="L22" s="15" t="s">
+      <c r="L22" s="14" t="s">
         <v>130</v>
       </c>
       <c r="M22" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="N22" s="23">
+      <c r="N22" s="20">
         <v>40.522661100000001</v>
       </c>
-      <c r="O22" s="23">
+      <c r="O22" s="20">
         <v>-105.0114408</v>
       </c>
-      <c r="P22" s="22" t="s">
+      <c r="P22" s="19" t="s">
         <v>173</v>
       </c>
       <c r="Q22" t="s">
@@ -4459,10 +4499,10 @@
       <c r="R22" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="S22" s="20" t="s">
+      <c r="S22" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="T22" s="20" t="s">
+      <c r="T22" s="18" t="s">
         <v>45</v>
       </c>
       <c r="U22" t="s">
@@ -4478,7 +4518,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="23" spans="1:24">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>40</v>
       </c>
@@ -4488,10 +4528,10 @@
       <c r="C23" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D23" s="20">
-        <v>20131179458</v>
-      </c>
-      <c r="E23" s="18" t="s">
+      <c r="D23" s="18" t="s">
+        <v>205</v>
+      </c>
+      <c r="E23" s="17" t="s">
         <v>45</v>
       </c>
       <c r="F23" t="s">
@@ -4512,19 +4552,19 @@
       <c r="K23" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="L23" s="15" t="s">
+      <c r="L23" s="14" t="s">
         <v>130</v>
       </c>
       <c r="M23" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="N23" s="23">
+      <c r="N23" s="20">
         <v>40.531162500000001</v>
       </c>
-      <c r="O23" s="23">
+      <c r="O23" s="20">
         <v>-105.0801891</v>
       </c>
-      <c r="P23" s="22" t="s">
+      <c r="P23" s="19" t="s">
         <v>173</v>
       </c>
       <c r="Q23" t="s">
@@ -4533,10 +4573,10 @@
       <c r="R23" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="S23" s="20" t="s">
+      <c r="S23" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="T23" s="20" t="s">
+      <c r="T23" s="18" t="s">
         <v>45</v>
       </c>
       <c r="U23" t="s">
@@ -4552,12 +4592,8 @@
         <v>146</v>
       </c>
     </row>
-    <row r="26" spans="1:24">
-      <c r="F26" s="9"/>
-    </row>
-    <row r="30" spans="1:24">
-      <c r="Q30" s="14"/>
-      <c r="R30" s="14"/>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="D24" s="13"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4597,7 +4633,7 @@
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="31.28515625" customWidth="1"/>
     <col min="2" max="2" width="21.140625" bestFit="1" customWidth="1"/>
@@ -4606,7 +4642,7 @@
     <col min="6" max="6" width="22.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>15</v>
       </c>
@@ -4626,21 +4662,21 @@
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>65</v>
       </c>
       <c r="B2" t="s">
         <v>102</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>128</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="12" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>92</v>
       </c>
@@ -4650,11 +4686,11 @@
       <c r="C3">
         <v>2014</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="11">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>92</v>
       </c>
@@ -4681,14 +4717,14 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.5703125" customWidth="1"/>
     <col min="2" max="2" width="27.28515625" customWidth="1"/>
     <col min="3" max="3" width="111.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4699,7 +4735,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>43118</v>
       </c>
@@ -4710,46 +4746,46 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3"/>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3"/>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3"/>
     </row>
   </sheetData>
@@ -4765,7 +4801,7 @@
       <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="99.28515625" bestFit="1" customWidth="1"/>
@@ -4773,7 +4809,7 @@
     <col min="5" max="5" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
@@ -4790,7 +4826,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -4807,7 +4843,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>17</v>
       </c>
@@ -4824,7 +4860,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>141</v>
       </c>
@@ -4841,7 +4877,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>18</v>
       </c>
@@ -4858,7 +4894,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>139</v>
       </c>
@@ -4875,7 +4911,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>121</v>
       </c>
@@ -4892,7 +4928,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -4909,7 +4945,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>26</v>
       </c>
@@ -4926,7 +4962,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>27</v>
       </c>
@@ -4943,7 +4979,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -4960,7 +4996,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>138</v>
       </c>
@@ -4977,7 +5013,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>25</v>
       </c>
@@ -4994,7 +5030,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>142</v>
       </c>
@@ -5011,7 +5047,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:5">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -5028,7 +5064,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:5">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -5045,7 +5081,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:5">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>144</v>
       </c>
@@ -5062,7 +5098,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -5079,7 +5115,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>162</v>
       </c>
@@ -5096,7 +5132,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -5113,7 +5149,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>161</v>
       </c>
@@ -5130,7 +5166,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -5147,7 +5183,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:5">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>147</v>
       </c>
@@ -5164,7 +5200,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>69</v>
       </c>
@@ -5181,7 +5217,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:5">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>175</v>
       </c>

</xml_diff>